<commit_message>
Updated Excel Sheet with Listed Operations Signed-off-by: anish30145784 <anish.mukherjee1@ucalgary.ca>
</commit_message>
<xml_diff>
--- a/Yash_MySQL_Queries/MySQL_Anish_Queries_MongoDB.xlsx
+++ b/Yash_MySQL_Queries/MySQL_Anish_Queries_MongoDB.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Downloads\ENSF603\Yash_MySQL_Queries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="194">
   <si>
     <t>Sr. No</t>
   </si>
@@ -509,6 +509,126 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE. MATCH, IN, GROUP, COUNT, SUM</t>
+  </si>
+  <si>
+    <t>AGGREGATE. GROUP, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE. GROUP, COUNT, SUM</t>
+  </si>
+  <si>
+    <t>AGGREGATE, MATCH, REGEX, OPTIONS, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, ADD, INDEXOFBYTES, ADDFIELDS, CONCAT, COND, IF, DATEFROMSTRING, MATCH, ISODATE, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, MATCH, EQ, GROUP, SUM</t>
+  </si>
+  <si>
+    <t>AGGREGATE ,MATCH, EQ, GROUP, COUNT, SUM</t>
+  </si>
+  <si>
+    <t>FIND, REGEX, OPTIONS, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, REGEX, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, GROUP, SUM</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, CEIL, DIVIDE, TOINT, SUBSTR, GROUP, SUM</t>
+  </si>
+  <si>
+    <t>FIND, EXPR, EQ, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, GROUP, SUM, SORT, LIMIT, ALLOWDISKUSE</t>
+  </si>
+  <si>
+    <t>AGGREGATE, MATCH, EXISTS, GROUP, ADDTOSET, PROJECT, SIZE, GT, SORT, LIMIT, ALLOWDISKUSE</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, GROUP, SUM</t>
+  </si>
+  <si>
+    <t>AGGREGATE, GROUP, SUM, MATCH, GT, PROJECT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, GROUP, SUM, MATCH, GT, COUNT, ALLOWDISKUSE</t>
+  </si>
+  <si>
+    <t>FIND, NOT, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, EXISTS, EXPR, GT, ADD, SUBSTRACT, STRLENCP, REPLACEALL, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, AND, NE, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, AND, REGEX, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, AND, REGEX, EXPR, GT, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE , PROJECT, TOINT, SUBSTR, SUBTRACT, STRLENCP, MATCH, LT, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, EXPR, LT, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, TOINT, SUBSTR, SUBTRACT, STRLENCP, ADDFIELDS, CONCAT, TOSTRING, GROUP, SUM, SORT, LIMIT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, ADD, INDEXOFBYTES, ADDFIELDS, CONCAT, COND, IF, EQ, THEN, ELSE, DATEFROMSTRING, ISODATE, MATCH, EXPR, AND, GTE, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, EXISTS, EXPR, GT, ADD, SUBTRACT, STRLENCP, REPLACEALL, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, AND, EXISTS, EXPR, GT, ADD, SUBTRACT, STRLENCP, REPLACEALL, EXPR, GTE, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, AND, EXISTS, EXPR, GT, ADD, SUBTRACT, STRLENCP, REPLACEALL, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, ADDFIELDS, TOINT, SUBSTR, SUBTRACT, STRLENCP, MATCH, AND, GT, COUNT</t>
+  </si>
+  <si>
+    <t>FIND, EXISTS, EXPR, GT, STRLENCP, COUNT</t>
+  </si>
+  <si>
+    <t>AGGREGATE, MATCH, NE, ADDFIELDS, COND, IF, EQ, STRLENCP, THEN, ELSE, GROUP, AVG</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, ADD, INDEXOFBYTES, DATEFROMSTRING, CONCAT, COND, IF, EQ, THEN, GROUP, MIN, MAX, ADDFIELDS, DIVIDE, MATCH, GT, LIMIT, ALLOWDISKUSE</t>
+  </si>
+  <si>
+    <t>AGGREGATE, GROUP, AVG</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, TOINT, SUBSTR, SUBTRACT, STRLENCP, GROUP, AVG</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, ADDFIELDS, CONCAT, GROUP, AVG</t>
+  </si>
+  <si>
+    <t>AGGREGATE, MATCH, NE, ADDFIELDS, TOINT, ADD, SUBTRACT, STRLENCP, REPLACEALL, GROUP, AVG</t>
+  </si>
+  <si>
+    <t>AGGREGATE, PROJECT, SUBSTR, SUBTRACT, STRLENCP, GROUP, SUM, SORT, LIMIT</t>
   </si>
 </sst>
 </file>
@@ -540,7 +660,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -685,19 +805,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FF000000"/>
@@ -706,21 +813,6 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -778,17 +870,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -826,21 +907,23 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -901,26 +984,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1024,6 +1098,61 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13214350" y="5457825"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1479550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522F2C51-26D5-46E1-9303-3B584FC1F200}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18735675" y="2971800"/>
           <a:ext cx="65" cy="172227"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2377,14 +2506,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="51.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9"/>
@@ -2393,96 +2522,93 @@
     <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.375" customWidth="1"/>
     <col min="9" max="11" width="18.375" customWidth="1"/>
-    <col min="12" max="12" width="17.5" customWidth="1"/>
-    <col min="13" max="13" width="23.5" customWidth="1"/>
+    <col min="12" max="12" width="56.375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="13" t="s">
         <v>105</v>
       </c>
       <c r="L1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    </row>
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>1</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="22">
         <v>1E-3</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="23">
         <v>1E-3</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="22">
         <v>1E-3</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="22">
         <v>1E-3</v>
       </c>
-      <c r="J2" s="27">
+      <c r="J2" s="24">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="22">
         <v>1E-3</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L2" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -2503,23 +2629,24 @@
       <c r="I3" s="15">
         <v>3.948</v>
       </c>
-      <c r="J3" s="28">
+      <c r="J3" s="25">
         <v>3.899</v>
       </c>
       <c r="K3" s="15">
         <v>3.7090000000000001</v>
       </c>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-    </row>
-    <row r="4" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L3" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -2540,23 +2667,24 @@
       <c r="I4" s="15">
         <v>3.2050000000000001</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="25">
         <v>2.9350000000000001</v>
       </c>
       <c r="K4" s="15">
         <v>2.4329999999999998</v>
       </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L4" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -2577,23 +2705,24 @@
       <c r="I5" s="15">
         <v>2.806</v>
       </c>
-      <c r="J5" s="28">
+      <c r="J5" s="25">
         <v>2.7709999999999999</v>
       </c>
       <c r="K5" s="15">
         <v>2.2799999999999998</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-    </row>
-    <row r="6" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="L5" s="15" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -2614,23 +2743,24 @@
       <c r="I6" s="15">
         <v>7.218</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="25">
         <v>6.7720000000000002</v>
       </c>
       <c r="K6" s="15">
         <v>5.8810000000000002</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-    </row>
-    <row r="7" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="L6" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -2651,23 +2781,24 @@
       <c r="I7" s="15">
         <v>5.96</v>
       </c>
-      <c r="J7" s="28">
+      <c r="J7" s="25">
         <v>5.3289999999999997</v>
       </c>
       <c r="K7" s="15">
         <v>4.5579999999999998</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-    </row>
-    <row r="8" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L7" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -2688,23 +2819,24 @@
       <c r="I8" s="15">
         <v>7.0609999999999999</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="25">
         <v>6.7960000000000003</v>
       </c>
       <c r="K8" s="15">
         <v>5.8250000000000002</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L8" s="15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D9" s="15" t="s">
@@ -2725,23 +2857,24 @@
       <c r="I9" s="15">
         <v>2.0739999999999998</v>
       </c>
-      <c r="J9" s="28">
+      <c r="J9" s="25">
         <v>1.7909999999999999</v>
       </c>
       <c r="K9" s="15">
         <v>1.508</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" ht="346.5" x14ac:dyDescent="0.25">
+      <c r="L9" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -2762,23 +2895,24 @@
       <c r="I10" s="15">
         <v>11.98</v>
       </c>
-      <c r="J10" s="28">
+      <c r="J10" s="25">
         <v>10.865</v>
       </c>
       <c r="K10" s="15">
         <v>9.0549999999999997</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-    </row>
-    <row r="11" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L10" s="15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -2799,23 +2933,24 @@
       <c r="I11" s="15">
         <v>3.613</v>
       </c>
-      <c r="J11" s="28">
+      <c r="J11" s="25">
         <v>3.1309999999999998</v>
       </c>
       <c r="K11" s="15">
         <v>2.5289999999999999</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-    </row>
-    <row r="12" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L11" s="15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -2836,23 +2971,24 @@
       <c r="I12" s="15">
         <v>2.6579999999999999</v>
       </c>
-      <c r="J12" s="28">
+      <c r="J12" s="25">
         <v>2.36</v>
       </c>
       <c r="K12" s="15">
         <v>2.0009999999999999</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-    </row>
-    <row r="13" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L12" s="15" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -2873,23 +3009,24 @@
       <c r="I13" s="15">
         <v>2.5369999999999999</v>
       </c>
-      <c r="J13" s="28">
+      <c r="J13" s="25">
         <v>2.323</v>
       </c>
       <c r="K13" s="15">
         <v>2.0179999999999998</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-    </row>
-    <row r="14" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L13" s="15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -2910,23 +3047,24 @@
       <c r="I14" s="15">
         <v>2.2480000000000002</v>
       </c>
-      <c r="J14" s="28">
+      <c r="J14" s="25">
         <v>2.0099999999999998</v>
       </c>
       <c r="K14" s="15">
         <v>1.772</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-    </row>
-    <row r="15" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="L14" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -2947,23 +3085,24 @@
       <c r="I15" s="15">
         <v>2.1429999999999998</v>
       </c>
-      <c r="J15" s="28">
+      <c r="J15" s="25">
         <v>1.857</v>
       </c>
       <c r="K15" s="15">
         <v>1.548</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-    </row>
-    <row r="16" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="L15" s="15" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -2984,23 +3123,24 @@
       <c r="I16" s="15">
         <v>3.524</v>
       </c>
-      <c r="J16" s="28">
+      <c r="J16" s="25">
         <v>3.306</v>
       </c>
       <c r="K16" s="15">
         <v>2.871</v>
       </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-    </row>
-    <row r="17" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="L16" s="15" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D17" s="15" t="s">
@@ -3021,23 +3161,24 @@
       <c r="I17" s="15">
         <v>4.3620000000000001</v>
       </c>
-      <c r="J17" s="28">
+      <c r="J17" s="25">
         <v>3.7320000000000002</v>
       </c>
       <c r="K17" s="15">
         <v>3.1509999999999998</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-    </row>
-    <row r="18" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L17" s="15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D18" s="15" t="s">
@@ -3058,23 +3199,24 @@
       <c r="I18" s="15">
         <v>3.4260000000000002</v>
       </c>
-      <c r="J18" s="28">
+      <c r="J18" s="25">
         <v>3.3410000000000002</v>
       </c>
       <c r="K18" s="15">
         <v>2.7410000000000001</v>
       </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-    </row>
-    <row r="19" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L18" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -3095,23 +3237,24 @@
       <c r="I19" s="15">
         <v>17.742000000000001</v>
       </c>
-      <c r="J19" s="28">
+      <c r="J19" s="25">
         <v>16.443000000000001</v>
       </c>
       <c r="K19" s="15">
         <v>14.712</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-    </row>
-    <row r="20" spans="1:13" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="L19" s="15" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -3132,23 +3275,24 @@
       <c r="I20" s="15">
         <v>26.067</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J20" s="25">
         <v>23.036000000000001</v>
       </c>
       <c r="K20" s="15">
         <v>22.611000000000001</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-    </row>
-    <row r="21" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="L20" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -3169,23 +3313,24 @@
       <c r="I21" s="15">
         <v>3.7930000000000001</v>
       </c>
-      <c r="J21" s="28">
+      <c r="J21" s="25">
         <v>3.319</v>
       </c>
       <c r="K21" s="15">
         <v>2.931</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-    </row>
-    <row r="22" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="L21" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D22" s="15" t="s">
@@ -3206,23 +3351,24 @@
       <c r="I22" s="15">
         <v>8.2080000000000002</v>
       </c>
-      <c r="J22" s="28">
+      <c r="J22" s="25">
         <v>7.17</v>
       </c>
       <c r="K22" s="15">
         <v>6.415</v>
       </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-    </row>
-    <row r="23" spans="1:13" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="L22" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D23" s="15" t="s">
@@ -3243,23 +3389,24 @@
       <c r="I23" s="15">
         <v>17.864000000000001</v>
       </c>
-      <c r="J23" s="28">
+      <c r="J23" s="25">
         <v>17.417000000000002</v>
       </c>
       <c r="K23" s="15">
         <v>14.738</v>
       </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-    </row>
-    <row r="24" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L23" s="15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -3280,23 +3427,24 @@
       <c r="I24" s="15">
         <v>3.4079999999999999</v>
       </c>
-      <c r="J24" s="28">
+      <c r="J24" s="25">
         <v>2.8780000000000001</v>
       </c>
       <c r="K24" s="15">
         <v>2.5369999999999999</v>
       </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="1:13" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L24" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D25" s="15" t="s">
@@ -3317,23 +3465,24 @@
       <c r="I25" s="15">
         <v>9.8469999999999995</v>
       </c>
-      <c r="J25" s="28">
+      <c r="J25" s="25">
         <v>8.702</v>
       </c>
       <c r="K25" s="15">
         <v>7.3280000000000003</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-    </row>
-    <row r="26" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L25" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D26" s="15" t="s">
@@ -3354,23 +3503,24 @@
       <c r="I26" s="15">
         <v>0.41899999999999998</v>
       </c>
-      <c r="J26" s="28">
+      <c r="J26" s="25">
         <v>0.39900000000000002</v>
       </c>
       <c r="K26" s="15">
         <v>0.34200000000000003</v>
       </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-    </row>
-    <row r="27" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="L26" s="15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D27" s="15" t="s">
@@ -3391,23 +3541,24 @@
       <c r="I27" s="15">
         <v>2.407</v>
       </c>
-      <c r="J27" s="28">
+      <c r="J27" s="25">
         <v>2.1360000000000001</v>
       </c>
       <c r="K27" s="15">
         <v>1.758</v>
       </c>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-    </row>
-    <row r="28" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L27" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D28" s="15" t="s">
@@ -3428,23 +3579,24 @@
       <c r="I28" s="15">
         <v>5.117</v>
       </c>
-      <c r="J28" s="28">
+      <c r="J28" s="25">
         <v>4.6470000000000002</v>
       </c>
       <c r="K28" s="15">
         <v>3.9409999999999998</v>
       </c>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-    </row>
-    <row r="29" spans="1:13" ht="63" x14ac:dyDescent="0.25">
+      <c r="L28" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D29" s="15" t="s">
@@ -3465,23 +3617,24 @@
       <c r="I29" s="15">
         <v>1.506</v>
       </c>
-      <c r="J29" s="28">
+      <c r="J29" s="25">
         <v>1.45</v>
       </c>
       <c r="K29" s="15">
         <v>1.248</v>
       </c>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-    </row>
-    <row r="30" spans="1:13" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="L29" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -3502,23 +3655,24 @@
       <c r="I30" s="15">
         <v>4.7720000000000002</v>
       </c>
-      <c r="J30" s="28">
+      <c r="J30" s="25">
         <v>4.423</v>
       </c>
       <c r="K30" s="15">
         <v>3.8410000000000002</v>
       </c>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-    </row>
-    <row r="31" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L30" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D31" s="15" t="s">
@@ -3539,23 +3693,24 @@
       <c r="I31" s="15">
         <v>2.0659999999999998</v>
       </c>
-      <c r="J31" s="28">
+      <c r="J31" s="25">
         <v>1.94</v>
       </c>
       <c r="K31" s="15">
         <v>1.6879999999999999</v>
       </c>
-      <c r="L31" s="14"/>
-      <c r="M31" s="14"/>
-    </row>
-    <row r="32" spans="1:13" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="L31" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -3576,23 +3731,24 @@
       <c r="I32" s="15">
         <v>7.0369999999999999</v>
       </c>
-      <c r="J32" s="28">
+      <c r="J32" s="25">
         <v>6.4580000000000002</v>
       </c>
       <c r="K32" s="15">
         <v>6.4640000000000004</v>
       </c>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-    </row>
-    <row r="33" spans="1:14" ht="362.25" x14ac:dyDescent="0.25">
+      <c r="L32" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D33" s="15" t="s">
@@ -3613,23 +3769,24 @@
       <c r="I33" s="15">
         <v>11.673</v>
       </c>
-      <c r="J33" s="28">
+      <c r="J33" s="25">
         <v>10.117000000000001</v>
       </c>
       <c r="K33" s="15">
         <v>9.8309999999999995</v>
       </c>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-    </row>
-    <row r="34" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="L33" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D34" s="15" t="s">
@@ -3650,23 +3807,24 @@
       <c r="I34" s="15">
         <v>5.9669999999999996</v>
       </c>
-      <c r="J34" s="28">
+      <c r="J34" s="25">
         <v>5.7430000000000003</v>
       </c>
       <c r="K34" s="15">
         <v>5.0720000000000001</v>
       </c>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-    </row>
-    <row r="35" spans="1:14" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L34" s="15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D35" s="15" t="s">
@@ -3687,23 +3845,24 @@
       <c r="I35" s="15">
         <v>17.28</v>
       </c>
-      <c r="J35" s="28">
+      <c r="J35" s="25">
         <v>15.167999999999999</v>
       </c>
       <c r="K35" s="15">
         <v>15.672000000000001</v>
       </c>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-    </row>
-    <row r="36" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L35" s="15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D36" s="15" t="s">
@@ -3724,23 +3883,24 @@
       <c r="I36" s="15">
         <v>4.8120000000000003</v>
       </c>
-      <c r="J36" s="28">
+      <c r="J36" s="25">
         <v>4.577</v>
       </c>
       <c r="K36" s="15">
         <v>3.6970000000000001</v>
       </c>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-    </row>
-    <row r="37" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L36" s="15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="25" t="s">
+      <c r="C37" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D37" s="15" t="s">
@@ -3761,23 +3921,24 @@
       <c r="I37" s="15">
         <v>14.625999999999999</v>
       </c>
-      <c r="J37" s="28">
+      <c r="J37" s="25">
         <v>12.351000000000001</v>
       </c>
       <c r="K37" s="15">
         <v>11.051</v>
       </c>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-    </row>
-    <row r="38" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L37" s="15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D38" s="15" t="s">
@@ -3798,23 +3959,24 @@
       <c r="I38" s="15">
         <v>9.3759999999999994</v>
       </c>
-      <c r="J38" s="28">
+      <c r="J38" s="25">
         <v>8.7970000000000006</v>
       </c>
       <c r="K38" s="15">
         <v>7.4080000000000004</v>
       </c>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-    </row>
-    <row r="39" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L38" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="25" t="s">
+      <c r="C39" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D39" s="15" t="s">
@@ -3835,24 +3997,25 @@
       <c r="I39" s="15">
         <v>6.2030000000000003</v>
       </c>
-      <c r="J39" s="28">
+      <c r="J39" s="25">
         <v>5.3070000000000004</v>
       </c>
       <c r="K39" s="15">
         <v>4.4800000000000004</v>
       </c>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="12"/>
-    </row>
-    <row r="40" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+      <c r="L39" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="M39" s="12"/>
+    </row>
+    <row r="40" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="25" t="s">
+      <c r="C40" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D40" s="15" t="s">
@@ -3873,23 +4036,24 @@
       <c r="I40" s="15">
         <v>5.7119999999999997</v>
       </c>
-      <c r="J40" s="28">
+      <c r="J40" s="25">
         <v>5.056</v>
       </c>
       <c r="K40" s="15">
         <v>4.1369999999999996</v>
       </c>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-    </row>
-    <row r="41" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L40" s="15" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="25" t="s">
+      <c r="C41" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D41" s="15" t="s">
@@ -3910,23 +4074,24 @@
       <c r="I41" s="15">
         <v>9.5570000000000004</v>
       </c>
-      <c r="J41" s="28">
+      <c r="J41" s="25">
         <v>9.3179999999999996</v>
       </c>
       <c r="K41" s="15">
         <v>7.5259999999999998</v>
       </c>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-    </row>
-    <row r="42" spans="1:14" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="L41" s="15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="25" t="s">
+      <c r="C42" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -3947,23 +4112,24 @@
       <c r="I42" s="15">
         <v>26.556000000000001</v>
       </c>
-      <c r="J42" s="28">
+      <c r="J42" s="25">
         <v>24.369</v>
       </c>
       <c r="K42" s="15">
         <v>25.306999999999999</v>
       </c>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-    </row>
-    <row r="43" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="L42" s="15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C43" s="25" t="s">
+      <c r="C43" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D43" s="15" t="s">
@@ -3984,23 +4150,24 @@
       <c r="I43" s="15">
         <v>3.2570000000000001</v>
       </c>
-      <c r="J43" s="28">
+      <c r="J43" s="25">
         <v>2.992</v>
       </c>
       <c r="K43" s="15">
         <v>2.4990000000000001</v>
       </c>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-    </row>
-    <row r="44" spans="1:14" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="L43" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="C44" s="25" t="s">
+      <c r="C44" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -4021,23 +4188,24 @@
       <c r="I44" s="15">
         <v>4.6849999999999996</v>
       </c>
-      <c r="J44" s="28">
+      <c r="J44" s="25">
         <v>4.343</v>
       </c>
       <c r="K44" s="15">
         <v>3.8279999999999998</v>
       </c>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-    </row>
-    <row r="45" spans="1:14" ht="157.5" x14ac:dyDescent="0.25">
+      <c r="L44" s="15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="25" t="s">
+      <c r="C45" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D45" s="15" t="s">
@@ -4058,23 +4226,24 @@
       <c r="I45" s="15">
         <v>6.4610000000000003</v>
       </c>
-      <c r="J45" s="28">
+      <c r="J45" s="25">
         <v>5.6440000000000001</v>
       </c>
       <c r="K45" s="15">
         <v>5.05</v>
       </c>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-    </row>
-    <row r="46" spans="1:14" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="L45" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="25" t="s">
+      <c r="C46" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D46" s="15" t="s">
@@ -4095,23 +4264,24 @@
       <c r="I46" s="15">
         <v>21.010999999999999</v>
       </c>
-      <c r="J46" s="28">
+      <c r="J46" s="25">
         <v>19.260000000000002</v>
       </c>
       <c r="K46" s="15">
         <v>19.257999999999999</v>
       </c>
-      <c r="L46" s="14"/>
-      <c r="M46" s="14"/>
-    </row>
-    <row r="47" spans="1:14" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="L46" s="15" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="25" t="s">
+      <c r="C47" s="22" t="s">
         <v>153</v>
       </c>
       <c r="D47" s="15" t="s">
@@ -4132,18 +4302,20 @@
       <c r="I47" s="15">
         <v>4.0609999999999999</v>
       </c>
-      <c r="J47" s="28">
+      <c r="J47" s="25">
         <v>3.7709999999999999</v>
       </c>
       <c r="K47" s="15">
         <v>3.2879999999999998</v>
       </c>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
+      <c r="L47" s="15" t="s">
+        <v>193</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add screenshots and updated excel sheet Signed-off-by: anish30145784 <anish.mukherjee1@ucalgary.ca>
</commit_message>
<xml_diff>
--- a/Yash_MySQL_Queries/MySQL_Anish_Queries_MongoDB.xlsx
+++ b/Yash_MySQL_Queries/MySQL_Anish_Queries_MongoDB.xlsx
@@ -2509,8 +2509,8 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>